<commit_message>
added STEP output, started working on 3D case
</commit_message>
<xml_diff>
--- a/cad/pcb/altium/outputs/esc/BOM/Bill of Materials-esc.xlsx
+++ b/cad/pcb/altium/outputs/esc/BOM/Bill of Materials-esc.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94F9B41C-9CBD-411A-B442-B3608F238563}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5590A9F-24B7-408B-9167-2922D8D859C5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{70645D7D-7B05-405A-AFB1-30BD884661ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{B714B232-63FE-43AD-96D1-691F6F32D1ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-esc" sheetId="1" r:id="rId1"/>
@@ -874,7 +874,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E323B9-C7FD-482A-AA74-563426C0B8B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE985677-A395-4529-ABBA-660682547167}">
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1756,64 +1756,64 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" tooltip="Manufacturer" display="'" xr:uid="{4A4FE004-F966-4E4A-AFAF-8DE4028C2215}"/>
-    <hyperlink ref="I2" tooltip="Supplier" display="'" xr:uid="{DE61773A-B56C-49EF-8010-15E59BD5BBC7}"/>
-    <hyperlink ref="F3" tooltip="Manufacturer" display="'" xr:uid="{7A85CCDB-968E-4745-A800-136510AA91B2}"/>
-    <hyperlink ref="I3" tooltip="Supplier" display="'" xr:uid="{65EB44F3-B731-417C-BDB8-7A350E20CE77}"/>
-    <hyperlink ref="F4" tooltip="Manufacturer" display="'" xr:uid="{A0AC10AE-C128-4511-AFFA-DFF9EB33C0F0}"/>
-    <hyperlink ref="I4" tooltip="Supplier" display="'" xr:uid="{C589118A-936E-48AA-8731-E1281DF02F4E}"/>
-    <hyperlink ref="F5" tooltip="Manufacturer" display="'" xr:uid="{00D9FB12-8117-4D8E-A096-50AD755BFA00}"/>
-    <hyperlink ref="I5" tooltip="Supplier" display="'" xr:uid="{E260A6C5-BB6E-4272-A38F-39C4478F10AA}"/>
-    <hyperlink ref="F6" r:id="rId1" tooltip="Manufacturer" display="'EEE-FK1V220R" xr:uid="{31CC622D-1828-47BF-AE6D-7B4EACD40C2C}"/>
-    <hyperlink ref="I6" r:id="rId2" tooltip="Supplier" display="'PCE3838DKR-ND" xr:uid="{8B51D39B-E7AB-4FBA-855B-981FBF863E62}"/>
-    <hyperlink ref="F7" r:id="rId3" tooltip="Manufacturer" display="'EEE-1VA221UP" xr:uid="{80095954-9118-4ABA-8460-67FAC48347EC}"/>
-    <hyperlink ref="I7" r:id="rId4" tooltip="Supplier" display="'PCE3955DKR-ND" xr:uid="{F1D5BFE4-3E11-4210-AB69-0294F639A2F2}"/>
-    <hyperlink ref="F8" tooltip="Manufacturer" display="'" xr:uid="{6077ED58-126B-4497-B2EE-1D3D9E6595CF}"/>
-    <hyperlink ref="I8" tooltip="Supplier" display="'" xr:uid="{835CD6AE-5EAF-4501-9EF7-916E961A736B}"/>
-    <hyperlink ref="F9" tooltip="Manufacturer" display="'" xr:uid="{151C3FD8-632C-45F9-A39C-994BAB508CF0}"/>
-    <hyperlink ref="I9" tooltip="Supplier" display="'" xr:uid="{14B821FA-2406-42EF-B0E4-CFC328D5F804}"/>
-    <hyperlink ref="F10" tooltip="Manufacturer" display="'" xr:uid="{FA0666D8-FE15-4A59-8B22-029645C82085}"/>
-    <hyperlink ref="I10" tooltip="Supplier" display="'" xr:uid="{701800EB-7BA8-42EA-99D5-2FB0950A021F}"/>
-    <hyperlink ref="F11" tooltip="Manufacturer" display="'" xr:uid="{392CC8A1-5873-4C8B-BBDB-9DAC685E6D20}"/>
-    <hyperlink ref="I11" tooltip="Supplier" display="'" xr:uid="{ADB1B61E-D428-4AB3-9A6B-D2FDA8F5959C}"/>
-    <hyperlink ref="F12" tooltip="Manufacturer" display="'" xr:uid="{3A3D7B4B-77B1-4BF1-8A17-DB1A585F1D33}"/>
-    <hyperlink ref="I12" tooltip="Supplier" display="'" xr:uid="{7A3BC5DF-4AE4-4B06-85AD-2A18326CB5FA}"/>
-    <hyperlink ref="F13" tooltip="Manufacturer" display="'" xr:uid="{131DFEAF-B1A7-4F54-8C6F-E6834CA5162D}"/>
-    <hyperlink ref="I13" tooltip="Supplier" display="'" xr:uid="{0AEFCB4C-0161-4BCA-9926-FE22F7427E84}"/>
-    <hyperlink ref="F14" tooltip="Manufacturer" display="'" xr:uid="{F8F3050E-5CC9-4B84-931E-5E7A2AF24CF5}"/>
-    <hyperlink ref="I14" tooltip="Supplier" display="'" xr:uid="{C03ADA4F-BE91-40CD-98F4-2CBE6A927200}"/>
-    <hyperlink ref="F15" r:id="rId5" tooltip="Manufacturer" display="'AOD4189" xr:uid="{50619037-96F5-42C0-A687-48E123E99D0E}"/>
-    <hyperlink ref="I15" r:id="rId6" tooltip="Supplier" display="'785-1351-6-ND" xr:uid="{966257CD-2DEC-43CB-9D62-D3DE70B2BB53}"/>
-    <hyperlink ref="F16" r:id="rId7" tooltip="Manufacturer" display="'STD35NF06LT4" xr:uid="{139770AB-3612-44FE-B2C2-73EAF73479AA}"/>
-    <hyperlink ref="I16" r:id="rId8" tooltip="Supplier" display="'497-7965-6-ND" xr:uid="{EF1D1560-113D-4A5E-B328-30B604B2D0C5}"/>
-    <hyperlink ref="F17" tooltip="Manufacturer" display="'" xr:uid="{B3903473-6A81-4DC5-9753-6F26658E9927}"/>
-    <hyperlink ref="I17" tooltip="Supplier" display="'" xr:uid="{EDB8FBF8-28CF-4229-B7D6-36CDB6C9E991}"/>
-    <hyperlink ref="F18" tooltip="Manufacturer" display="'" xr:uid="{E2359A30-8F33-4C39-972B-A2256BF6856E}"/>
-    <hyperlink ref="I18" tooltip="Supplier" display="'" xr:uid="{9CEFD5B9-D44B-4DB3-BD37-F2E13D9D5861}"/>
-    <hyperlink ref="F19" tooltip="Manufacturer" display="'" xr:uid="{3FCDEB39-7C41-4D10-9BCC-08556924F25B}"/>
-    <hyperlink ref="I19" tooltip="Supplier" display="'" xr:uid="{603630AC-8D18-4111-85FB-CE7C3110CD1F}"/>
-    <hyperlink ref="F20" r:id="rId9" tooltip="Manufacturer" display="'CSR1206-0R001F1" xr:uid="{8E29F7AC-8C9E-4857-9C74-5AD06664B8C0}"/>
-    <hyperlink ref="I20" r:id="rId10" tooltip="Supplier" display="'696-1369-6-ND" xr:uid="{90575ED6-B57B-4C38-8D50-2CC54B9DA80C}"/>
-    <hyperlink ref="F21" tooltip="Manufacturer" display="'" xr:uid="{061DEC71-5F88-4519-8966-C78D82684EC3}"/>
-    <hyperlink ref="I21" tooltip="Supplier" display="'" xr:uid="{A124BB20-0F5E-4C53-8367-0E1E319A5175}"/>
-    <hyperlink ref="F22" tooltip="Manufacturer" display="'" xr:uid="{CF08877E-EDFC-4F3C-8E45-EAFDB733501D}"/>
-    <hyperlink ref="I22" tooltip="Supplier" display="'" xr:uid="{8784C2CA-FF12-458F-8A85-7CAAD1FC4661}"/>
-    <hyperlink ref="F23" r:id="rId11" tooltip="Manufacturer" display="'219-5LPST" xr:uid="{93FEB03C-D816-4037-B36A-7C06AAC71664}"/>
-    <hyperlink ref="I23" r:id="rId12" tooltip="Supplier" display="'CT2195LPST-ND" xr:uid="{D310190E-F737-4EDA-AB9C-8172C11514B6}"/>
-    <hyperlink ref="F24" r:id="rId13" tooltip="Manufacturer" display="'1625854-3" xr:uid="{4A7DEFAA-A7A0-4C8C-AFB6-63E7A2DAE4EB}"/>
-    <hyperlink ref="I24" r:id="rId14" tooltip="Supplier" display="'A106145DKR-ND" xr:uid="{737CF2AA-185B-448D-B998-74EE1E794CA9}"/>
-    <hyperlink ref="F25" r:id="rId15" tooltip="Manufacturer" display="'TB6575FNG,C,8,EL" xr:uid="{6D9680EE-B814-4169-8025-1E171EB2A445}"/>
-    <hyperlink ref="I25" r:id="rId16" tooltip="Supplier" display="'TB6575FNGC8ELDKR-ND" xr:uid="{F2E0AB5E-61D3-4794-BA70-8F3DA169799D}"/>
-    <hyperlink ref="F26" r:id="rId17" tooltip="Manufacturer" display="'MCP14A0052T-E/CH" xr:uid="{A32F6150-3BFF-4A87-BB6D-694B605155AF}"/>
-    <hyperlink ref="I26" r:id="rId18" tooltip="Supplier" display="'MCP14A0052T-E/CHDKR-ND" xr:uid="{652C52EE-93F7-4B0D-A5B5-ACB4C16C8FB2}"/>
-    <hyperlink ref="F27" r:id="rId19" tooltip="Manufacturer" display="'INA199A1DCKR" xr:uid="{BFAAF928-2617-40F4-8C28-8D9F3B55DBE6}"/>
-    <hyperlink ref="I27" r:id="rId20" tooltip="Supplier" display="'296-27329-6-ND" xr:uid="{C7D8716B-876B-4015-9928-E43BE6D2C75B}"/>
-    <hyperlink ref="F28" r:id="rId21" tooltip="Manufacturer" display="'LMC7221BIM5X/NOPB" xr:uid="{8BCEECF8-15C4-4F48-8C9E-D098E4E013D9}"/>
-    <hyperlink ref="I28" r:id="rId22" tooltip="Supplier" display="'LMC7221BIM5X/NOPBDKR-ND" xr:uid="{CC48F762-AEBF-4B68-9472-DB2123570DEC}"/>
-    <hyperlink ref="F29" r:id="rId23" tooltip="Manufacturer" display="'L78L05ACUTR" xr:uid="{193D328E-7F84-47FF-A903-604EB32A6E71}"/>
-    <hyperlink ref="I29" r:id="rId24" tooltip="Supplier" display="'497-1183-6-ND" xr:uid="{BE1E427B-3651-4655-B9FA-C91D4F1A6FE8}"/>
-    <hyperlink ref="F30" r:id="rId25" tooltip="Manufacturer" display="'CSTCR4M19G53-R0" xr:uid="{3CD71103-F856-4FEA-878B-49905CF20D2E}"/>
-    <hyperlink ref="I30" r:id="rId26" tooltip="Supplier" display="'490-1201-6-ND" xr:uid="{720D7EDE-AC99-4217-A048-8C082CB3CDF8}"/>
+    <hyperlink ref="F2" tooltip="Manufacturer" display="'" xr:uid="{B02A8AE3-F1B2-477A-A0E4-4EB781CB2C1B}"/>
+    <hyperlink ref="I2" tooltip="Supplier" display="'" xr:uid="{E75FDF8D-BB90-41C6-BC2B-7861C9C7B7C9}"/>
+    <hyperlink ref="F3" tooltip="Manufacturer" display="'" xr:uid="{619282E4-9255-4B16-B609-321ADF393071}"/>
+    <hyperlink ref="I3" tooltip="Supplier" display="'" xr:uid="{8D66DC79-CF23-4391-8DD0-F51BD9D674A1}"/>
+    <hyperlink ref="F4" tooltip="Manufacturer" display="'" xr:uid="{602467FF-170E-416E-B022-9C2A793CF29D}"/>
+    <hyperlink ref="I4" tooltip="Supplier" display="'" xr:uid="{236B4C5D-6CBA-4B0C-9513-2D540C319BA7}"/>
+    <hyperlink ref="F5" tooltip="Manufacturer" display="'" xr:uid="{809FCA06-ABC2-45FB-B52C-D3F19BEA2185}"/>
+    <hyperlink ref="I5" tooltip="Supplier" display="'" xr:uid="{ACC8C8F6-AA34-4D5D-B947-66931845B124}"/>
+    <hyperlink ref="F6" r:id="rId1" tooltip="Manufacturer" display="'EEE-FK1V220R" xr:uid="{CD94F7BE-89B4-4666-99F2-4AFDD7642D6F}"/>
+    <hyperlink ref="I6" r:id="rId2" tooltip="Supplier" display="'PCE3838DKR-ND" xr:uid="{42CADF41-5C56-47BB-8945-B4A9166A9F0E}"/>
+    <hyperlink ref="F7" r:id="rId3" tooltip="Manufacturer" display="'EEE-1VA221UP" xr:uid="{E0A5DB50-DFC7-4306-BFE5-F7E47BB7A1DB}"/>
+    <hyperlink ref="I7" r:id="rId4" tooltip="Supplier" display="'PCE3955DKR-ND" xr:uid="{261B8D32-F5C6-4F3F-9EB7-92CD4E5444ED}"/>
+    <hyperlink ref="F8" tooltip="Manufacturer" display="'" xr:uid="{C133B1D8-E325-4739-8ACC-817179B64A13}"/>
+    <hyperlink ref="I8" tooltip="Supplier" display="'" xr:uid="{8146101D-A294-4E4A-81FF-814494283292}"/>
+    <hyperlink ref="F9" tooltip="Manufacturer" display="'" xr:uid="{AD22D0C6-9457-484A-9225-9EDE256EF037}"/>
+    <hyperlink ref="I9" tooltip="Supplier" display="'" xr:uid="{FF29D20E-93ED-47EE-A9AE-16B42EDD5FA5}"/>
+    <hyperlink ref="F10" tooltip="Manufacturer" display="'" xr:uid="{83300B2F-C18C-4292-BCDC-AA89A0631A20}"/>
+    <hyperlink ref="I10" tooltip="Supplier" display="'" xr:uid="{4B45AAAF-CD6D-4A8F-B188-987D19F62FC0}"/>
+    <hyperlink ref="F11" tooltip="Manufacturer" display="'" xr:uid="{59F9B75A-691B-464F-BA85-0C77AFDB2145}"/>
+    <hyperlink ref="I11" tooltip="Supplier" display="'" xr:uid="{AA245CC7-66AE-4D72-A679-5DD5F3C1C441}"/>
+    <hyperlink ref="F12" tooltip="Manufacturer" display="'" xr:uid="{E05BE95D-7089-41FA-9394-4E8C3D734F6D}"/>
+    <hyperlink ref="I12" tooltip="Supplier" display="'" xr:uid="{E8AC9043-C085-43C9-947F-546C412C1124}"/>
+    <hyperlink ref="F13" tooltip="Manufacturer" display="'" xr:uid="{141A3B63-97AA-4E57-B162-F95D3407A612}"/>
+    <hyperlink ref="I13" tooltip="Supplier" display="'" xr:uid="{69094CED-AA12-4378-A51F-B9192BD9E7F9}"/>
+    <hyperlink ref="F14" tooltip="Manufacturer" display="'" xr:uid="{5697DDE1-2F70-4366-82A1-9890DDEDC41F}"/>
+    <hyperlink ref="I14" tooltip="Supplier" display="'" xr:uid="{42553044-55E0-4ED9-8C8C-7BF6347F5EBE}"/>
+    <hyperlink ref="F15" r:id="rId5" tooltip="Manufacturer" display="'AOD4189" xr:uid="{E4902778-D240-4BEB-B1CB-F85544A45C37}"/>
+    <hyperlink ref="I15" r:id="rId6" tooltip="Supplier" display="'785-1351-6-ND" xr:uid="{2F0A1214-9E70-476B-86A9-7774B4116E73}"/>
+    <hyperlink ref="F16" r:id="rId7" tooltip="Manufacturer" display="'STD35NF06LT4" xr:uid="{22D19D8A-DE0D-40A1-A855-057FDCB73E05}"/>
+    <hyperlink ref="I16" r:id="rId8" tooltip="Supplier" display="'497-7965-6-ND" xr:uid="{7CFB1F6A-333F-4407-854E-886C01D223A8}"/>
+    <hyperlink ref="F17" tooltip="Manufacturer" display="'" xr:uid="{7D2912A3-CFE9-4F2B-8BAB-DA0ED5DF1436}"/>
+    <hyperlink ref="I17" tooltip="Supplier" display="'" xr:uid="{5D3B48BB-A2D4-4E24-BD14-AFBC91B7BF77}"/>
+    <hyperlink ref="F18" tooltip="Manufacturer" display="'" xr:uid="{1F503139-8A7E-4D26-AC39-30DD335F371C}"/>
+    <hyperlink ref="I18" tooltip="Supplier" display="'" xr:uid="{30823C2E-7055-4828-A097-AAB982754812}"/>
+    <hyperlink ref="F19" tooltip="Manufacturer" display="'" xr:uid="{DD126756-9DE6-442E-A755-531D21AF6A84}"/>
+    <hyperlink ref="I19" tooltip="Supplier" display="'" xr:uid="{938BC320-973A-4A87-9E59-373254545072}"/>
+    <hyperlink ref="F20" r:id="rId9" tooltip="Manufacturer" display="'CSR1206-0R001F1" xr:uid="{A49F1D54-9BE1-477F-9F52-65CE182073D7}"/>
+    <hyperlink ref="I20" r:id="rId10" tooltip="Supplier" display="'696-1369-6-ND" xr:uid="{1BCA6AE7-D2C4-4D18-AD41-F58865989AB5}"/>
+    <hyperlink ref="F21" tooltip="Manufacturer" display="'" xr:uid="{05CC703C-8EFE-44F0-A2D9-4E8E14E2D5B1}"/>
+    <hyperlink ref="I21" tooltip="Supplier" display="'" xr:uid="{1B948ADE-6888-4723-AEE3-FA4F81187D27}"/>
+    <hyperlink ref="F22" tooltip="Manufacturer" display="'" xr:uid="{8F109E3B-D430-482F-A190-B1E8BB3D5C6F}"/>
+    <hyperlink ref="I22" tooltip="Supplier" display="'" xr:uid="{F6DAEFBF-0178-4564-8C56-B626E0448CD4}"/>
+    <hyperlink ref="F23" r:id="rId11" tooltip="Manufacturer" display="'219-5LPST" xr:uid="{93C6D1D1-9314-4B11-BED8-3EF75AACF599}"/>
+    <hyperlink ref="I23" r:id="rId12" tooltip="Supplier" display="'CT2195LPST-ND" xr:uid="{82778B34-7947-4243-ABDE-3EFE68262E8A}"/>
+    <hyperlink ref="F24" r:id="rId13" tooltip="Manufacturer" display="'1625854-3" xr:uid="{1E9F3B2E-964D-47B9-874F-963E5BEDABF2}"/>
+    <hyperlink ref="I24" r:id="rId14" tooltip="Supplier" display="'A106145DKR-ND" xr:uid="{E79FE463-73A9-4A08-A2AE-C36DAA57B385}"/>
+    <hyperlink ref="F25" r:id="rId15" tooltip="Manufacturer" display="'TB6575FNG,C,8,EL" xr:uid="{876D4637-36F9-43BF-9792-946AFCBC306B}"/>
+    <hyperlink ref="I25" r:id="rId16" tooltip="Supplier" display="'TB6575FNGC8ELDKR-ND" xr:uid="{231014F7-AFF9-4A9B-AB09-FE608383A9AF}"/>
+    <hyperlink ref="F26" r:id="rId17" tooltip="Manufacturer" display="'MCP14A0052T-E/CH" xr:uid="{8BC0D4CB-87F7-463E-850E-2ACF3A7575A9}"/>
+    <hyperlink ref="I26" r:id="rId18" tooltip="Supplier" display="'MCP14A0052T-E/CHDKR-ND" xr:uid="{D1803892-15C8-4CE7-A597-3CDD9BE8776B}"/>
+    <hyperlink ref="F27" r:id="rId19" tooltip="Manufacturer" display="'INA199A1DCKR" xr:uid="{4B53EC6B-9478-41A9-A6F3-1D240AEC47BA}"/>
+    <hyperlink ref="I27" r:id="rId20" tooltip="Supplier" display="'296-27329-6-ND" xr:uid="{B3779019-217D-434C-875B-8B1830A59164}"/>
+    <hyperlink ref="F28" r:id="rId21" tooltip="Manufacturer" display="'LMC7221BIM5X/NOPB" xr:uid="{DFD9AB57-5158-4EEB-8843-1CD8CE56ECEC}"/>
+    <hyperlink ref="I28" r:id="rId22" tooltip="Supplier" display="'LMC7221BIM5X/NOPBDKR-ND" xr:uid="{9A964A6B-1843-42E5-9FB5-7F99DE63ABAB}"/>
+    <hyperlink ref="F29" r:id="rId23" tooltip="Manufacturer" display="'L78L05ACUTR" xr:uid="{96E57698-5330-4859-A261-496AAB4CA93F}"/>
+    <hyperlink ref="I29" r:id="rId24" tooltip="Supplier" display="'497-1183-6-ND" xr:uid="{3ABB987A-52C3-473E-87DD-21DE3B677AA3}"/>
+    <hyperlink ref="F30" r:id="rId25" tooltip="Manufacturer" display="'CSTCR4M19G53-R0" xr:uid="{E4A6A6C9-D416-4082-A513-96FB2D7EFC32}"/>
+    <hyperlink ref="I30" r:id="rId26" tooltip="Supplier" display="'490-1201-6-ND" xr:uid="{39D57A30-6E07-423D-95BD-9D9FB25F20D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId27"/>

</xml_diff>